<commit_message>
alteracao da maquina de estados
</commit_message>
<xml_diff>
--- a/lab3/estados.xlsx
+++ b/lab3/estados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="282" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="567" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
   <si>
     <t>MR_addr</t>
   </si>
@@ -62,12 +62,12 @@
     <t>ler linha 3</t>
   </si>
   <si>
+    <t>colocar oper em todos os registos</t>
+  </si>
+  <si>
     <t>shift</t>
   </si>
   <si>
-    <t>colocar oper em todos os registos</t>
-  </si>
-  <si>
     <t>res0</t>
   </si>
   <si>
@@ -86,16 +86,7 @@
     <t>s_process</t>
   </si>
   <si>
-    <t>s_last0</t>
-  </si>
-  <si>
-    <t>s_last1</t>
-  </si>
-  <si>
-    <t>s_last2</t>
-  </si>
-  <si>
-    <t>s_write (ainda nazo esta implementado)</t>
+    <t>s_last</t>
   </si>
   <si>
     <t>s_end</t>
@@ -113,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -134,6 +126,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,12 +137,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -195,23 +195,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -234,8 +234,8 @@
   </sheetPr>
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y4" activeCellId="0" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -508,34 +508,34 @@
         <v>111</v>
       </c>
       <c r="R3" s="2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S3" s="2" t="n">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="T3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="U3" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AB3" s="2" t="n">
         <v>0</v>
@@ -598,31 +598,31 @@
         <v>0</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>1</v>
+      <c r="U4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AB4" s="2" t="n">
         <v>0</v>
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" s="2" t="n">
         <v>0</v>
@@ -694,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="2" t="n">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6" s="2" t="n">
         <v>0</v>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="V6" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="2" t="n">
         <v>0</v>
@@ -859,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7" s="2" t="n">
         <v>0</v>
@@ -868,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="V7" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="2" t="n">
         <v>0</v>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="T8" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="2" t="n">
         <v>0</v>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="W8" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" s="2" t="n">
         <v>0</v>
@@ -1277,35 +1277,32 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="0" t="s">
-        <v>15</v>
-      </c>
+      <c r="R12" s="5"/>
       <c r="T12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>18</v>
@@ -1313,56 +1310,53 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T13" s="3" t="s">
+      <c r="V13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W13" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="7" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S14" s="7" t="s">
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="T14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1373,8 +1367,8 @@
     <mergeCell ref="N12:Q12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:Q14"/>
-    <mergeCell ref="U14:AA14"/>
+    <mergeCell ref="F14:U14"/>
+    <mergeCell ref="V14:AA14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>